<commit_message>
End profil Pro et admin
</commit_message>
<xml_diff>
--- a/racoin-backlog-initial/prioriteRacoin.xlsx
+++ b/racoin-backlog-initial/prioriteRacoin.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
   <si>
     <t>Stories</t>
   </si>
@@ -30,14 +30,119 @@
     <t>ok</t>
   </si>
   <si>
-    <t>Erreur</t>
+    <t>Pas à faire</t>
+  </si>
+  <si>
+    <t>Descrption</t>
+  </si>
+  <si>
+    <t>Indiquer un n° d'annonce dans l'url</t>
+  </si>
+  <si>
+    <t>Cliquer sur la photo en miniature</t>
+  </si>
+  <si>
+    <t>Voir toutes les annonce</t>
+  </si>
+  <si>
+    <t>Selectionner une annonce</t>
+  </si>
+  <si>
+    <t>entrer une catég dans l'url</t>
+  </si>
+  <si>
+    <t>ajouter une annonce</t>
+  </si>
+  <si>
+    <t>ajouter une photo en creant une annonce</t>
+  </si>
+  <si>
+    <t>Prévisualiser une annonce</t>
+  </si>
+  <si>
+    <t>obtenir les coordonnées de l'annonceur</t>
+  </si>
+  <si>
+    <t>supprimer une de ms annonce</t>
+  </si>
+  <si>
+    <t>modifier une annonce</t>
+  </si>
+  <si>
+    <t>acceder à la lister de mes annonces</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>chercher annonce par categ</t>
+  </si>
+  <si>
+    <t>chercher annonce selon tarif</t>
+  </si>
+  <si>
+    <t>chercher un terme dans le titre ou descr</t>
+  </si>
+  <si>
+    <t>combiner les 3 critères de recherches</t>
+  </si>
+  <si>
+    <t>admin : créer un compte admin</t>
+  </si>
+  <si>
+    <t>REST : liste annonce JSON</t>
+  </si>
+  <si>
+    <t>REST : liste categ JSON</t>
+  </si>
+  <si>
+    <t>REST : descr d'une annonce JSON</t>
+  </si>
+  <si>
+    <t>REST : liste annonce d'une categ JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REST : modif annonce </t>
+  </si>
+  <si>
+    <t>A faire</t>
+  </si>
+  <si>
+    <t>REST : ajout annonce</t>
+  </si>
+  <si>
+    <t>REST : liste avec filtre</t>
+  </si>
+  <si>
+    <t>admin : ajouter cat</t>
+  </si>
+  <si>
+    <t>pro : créer compte</t>
+  </si>
+  <si>
+    <t>pro : ajouter annonce</t>
+  </si>
+  <si>
+    <t>pro : afficher profil</t>
+  </si>
+  <si>
+    <t>pro : liste annonce</t>
+  </si>
+  <si>
+    <t>Fait ?</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Thomas + Jean-Noel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,13 +150,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,238 +531,570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" activeCellId="1" sqref="A18 A19"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="42.125" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
         <f t="shared" ref="A4:A19" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
         <f>A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
         <f>A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="D19" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="3">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>